<commit_message>
Don’t crash when a user has no rider object.  Return all race licences from the database in the downloaded spreadsheet.
</commit_message>
<xml_diff>
--- a/races/apps/cabici/tests/Waratahresults201536.xlsx
+++ b/races/apps/cabici/tests/Waratahresults201536.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/projects/races/races/apps/site/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/projects/races/races/apps/cabici/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5009,7 +5009,7 @@
         <v>17</v>
       </c>
       <c r="G98" s="3">
-        <v>81</v>
+        <v>999</v>
       </c>
       <c r="H98" s="2">
         <v>2</v>

</xml_diff>